<commit_message>
Update on 2023.12.14. 20:27
</commit_message>
<xml_diff>
--- a/llm_babysitting/data/task_1/result.xlsx
+++ b/llm_babysitting/data/task_1/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LeeYuseop\OneDrive\바탕 화면\Lecture\2023-2\2023-2 Natural Language Processing (001)\project\LLM_Babysitting_Project\llm_babysitting\data\task_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{0E147D2A-360D-4506-9111-427BB15BE8B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{4B4DE052-CD37-4D02-8209-65056CC51A3D}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{0E147D2A-360D-4506-9111-427BB15BE8B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{CECDEFCC-6F83-4C64-8F88-BC2930A1CAFD}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>답</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,6 +57,10 @@
   </si>
   <si>
     <t>7_7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6_6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -481,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X32"/>
+  <dimension ref="A1:AB32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -499,11 +503,14 @@
     <col min="14" max="14" width="9.5" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="8.6640625" style="3"/>
     <col min="17" max="17" width="8.6640625" style="2"/>
-    <col min="18" max="18" width="8.6640625" style="3"/>
-    <col min="19" max="19" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="8.6640625" style="3"/>
+    <col min="21" max="21" width="8.6640625" style="2"/>
+    <col min="22" max="22" width="8.6640625" style="3"/>
+    <col min="23" max="23" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
       <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
@@ -516,8 +523,11 @@
       <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="R1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="3">
         <v>1</v>
@@ -555,16 +565,25 @@
       <c r="P2" s="3">
         <v>3</v>
       </c>
-      <c r="S2" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="R2" s="3">
+        <v>1</v>
+      </c>
+      <c r="S2" s="3">
+        <v>2</v>
+      </c>
+      <c r="T2" s="3">
+        <v>3</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="str">
-        <f>IF(COUNT(B3:D3) &lt;&gt; 0, SUM(B3:D3)/COUNT(B3:D3), "-%")</f>
+        <f t="shared" ref="E3:E32" si="0">IF(COUNT(B3:D3) &lt;&gt; 0, SUM(B3:D3)/COUNT(B3:D3), "-%")</f>
         <v>-%</v>
       </c>
       <c r="I3" s="2" t="str">
@@ -579,31 +598,35 @@
         <f>IF(COUNT(N3:P3) &lt;&gt; 0, SUM(N3:P3)/COUNT(N3:P3), "-%")</f>
         <v>-%</v>
       </c>
-      <c r="S3" s="3">
-        <v>0</v>
-      </c>
-      <c r="T3" s="2">
-        <v>0</v>
-      </c>
-      <c r="U3" t="s">
+      <c r="U3" s="2" t="str">
+        <f>IF(COUNT(R3:T3) &lt;&gt; 0, SUM(R3:T3)/COUNT(R3:T3), "-%")</f>
+        <v>-%</v>
+      </c>
+      <c r="W3" s="3">
+        <v>0</v>
+      </c>
+      <c r="X3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="s">
         <v>2</v>
       </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="E4" s="2" t="str">
-        <f>IF(COUNT(B4:D4) &lt;&gt; 0, SUM(B4:D4)/COUNT(B4:D4), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F4">
@@ -616,7 +639,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" ref="I4:I32" si="0">IF(COUNT(F4:H4) &lt;&gt; 0, SUM(F4:H4)/COUNT(F4:H4), "-%")</f>
+        <f t="shared" ref="I4:I32" si="1">IF(COUNT(F4:H4) &lt;&gt; 0, SUM(F4:H4)/COUNT(F4:H4), "-%")</f>
         <v>0</v>
       </c>
       <c r="J4" s="3">
@@ -629,36 +652,46 @@
         <v>0</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" ref="M4:M32" si="1">IF(COUNT(J4:L4) &lt;&gt; 0, SUM(J4:L4)/COUNT(J4:L4), "-%")</f>
+        <f t="shared" ref="M4:M32" si="2">IF(COUNT(J4:L4) &lt;&gt; 0, SUM(J4:L4)/COUNT(J4:L4), "-%")</f>
         <v>0</v>
       </c>
       <c r="N4" s="3">
         <v>0</v>
       </c>
       <c r="Q4" s="2">
-        <f t="shared" ref="Q4:Q32" si="2">IF(COUNT(N4:P4) &lt;&gt; 0, SUM(N4:P4)/COUNT(N4:P4), "-%")</f>
+        <f t="shared" ref="Q4:Q32" si="3">IF(COUNT(N4:P4) &lt;&gt; 0, SUM(N4:P4)/COUNT(N4:P4), "-%")</f>
         <v>0</v>
       </c>
       <c r="S4" s="3">
+        <v>0</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0</v>
+      </c>
+      <c r="U4" s="2">
+        <f t="shared" ref="U4:U32" si="4">IF(COUNT(R4:T4) &lt;&gt; 0, SUM(R4:T4)/COUNT(R4:T4), "-%")</f>
+        <v>0</v>
+      </c>
+      <c r="W4" s="3">
         <v>101.063887103762</v>
       </c>
-      <c r="T4" s="2">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
       <c r="X4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -666,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <f>IF(COUNT(B5:D5) &lt;&gt; 0, SUM(B5:D5)/COUNT(B5:D5), "-%")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F5">
@@ -679,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K5" s="3">
@@ -689,7 +722,7 @@
         <v>1</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N5" s="3">
@@ -702,29 +735,36 @@
         <v>1</v>
       </c>
       <c r="Q5" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="S5" s="3">
+        <v>1</v>
+      </c>
+      <c r="U5" s="2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="W5" s="3">
         <v>-1100</v>
       </c>
-      <c r="T5" s="2">
-        <v>1</v>
-      </c>
-      <c r="U5">
-        <v>1</v>
-      </c>
-      <c r="V5">
-        <v>1</v>
-      </c>
-      <c r="W5">
-        <v>1</v>
-      </c>
       <c r="X5" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -735,7 +775,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <f>IF(COUNT(B6:D6) &lt;&gt; 0, SUM(B6:D6)/COUNT(B6:D6), "-%")</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="F6">
@@ -748,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J6" s="3">
@@ -761,81 +801,95 @@
         <v>1</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="Q6" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-%</v>
       </c>
       <c r="S6" s="3">
+        <v>1</v>
+      </c>
+      <c r="T6" s="3">
+        <v>0</v>
+      </c>
+      <c r="U6" s="2">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="W6" s="3">
         <v>0.99999821052946403</v>
       </c>
-      <c r="T6" s="2">
+      <c r="X6" s="2">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>1</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="X6" s="2">
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="2">
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="E7" s="2" t="str">
-        <f>IF(COUNT(B7:D7) &lt;&gt; 0, SUM(B7:D7)/COUNT(B7:D7), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M7" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q7" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S7" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U7" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W7" s="3">
         <v>10</v>
       </c>
-      <c r="T7" s="2">
-        <v>1</v>
-      </c>
-      <c r="U7">
-        <v>1</v>
-      </c>
-      <c r="V7">
-        <v>1</v>
-      </c>
-      <c r="W7">
-        <v>1</v>
-      </c>
       <c r="X7" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="E8" s="2" t="str">
-        <f>IF(COUNT(B8:D8) &lt;&gt; 0, SUM(B8:D8)/COUNT(B8:D8), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F8">
@@ -848,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J8" s="3">
@@ -861,38 +915,42 @@
         <v>0</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q8" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S8" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U8" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W8" s="3">
         <v>-19.925572692579401</v>
       </c>
-      <c r="T8" s="2">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
       <c r="X8" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="E9" s="2" t="str">
-        <f>IF(COUNT(B9:D9) &lt;&gt; 0, SUM(B9:D9)/COUNT(B9:D9), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F9">
@@ -905,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J9" s="3">
@@ -915,33 +973,37 @@
         <v>0</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q9" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S9" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U9" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W9" s="3">
         <v>-95101717.5</v>
       </c>
-      <c r="T9" s="2">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
       <c r="X9" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>8</v>
       </c>
@@ -949,7 +1011,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <f>IF(COUNT(B10:D10) &lt;&gt; 0, SUM(B10:D10)/COUNT(B10:D10), "-%")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10">
@@ -962,40 +1024,44 @@
         <v>0</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K10" s="3">
         <v>0</v>
       </c>
       <c r="M10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q10" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S10" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U10" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W10" s="3">
         <v>1.0131995858107601</v>
       </c>
-      <c r="T10" s="2">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="W10">
-        <v>0</v>
-      </c>
       <c r="X10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1006,7 +1072,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="2">
-        <f>IF(COUNT(B11:D11) &lt;&gt; 0, SUM(B11:D11)/COUNT(B11:D11), "-%")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F11">
@@ -1019,45 +1085,49 @@
         <v>1</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J11" s="3">
         <v>1</v>
       </c>
       <c r="M11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q11" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S11" s="3">
-        <v>0</v>
-      </c>
-      <c r="T11" s="2">
-        <v>1</v>
-      </c>
-      <c r="U11">
-        <v>1</v>
-      </c>
-      <c r="V11">
-        <v>1</v>
-      </c>
-      <c r="W11">
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U11" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W11" s="3">
+        <v>0</v>
       </c>
       <c r="X11" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <v>1</v>
+      </c>
+      <c r="AA11">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="E12" s="2" t="str">
-        <f>IF(COUNT(B12:D12) &lt;&gt; 0, SUM(B12:D12)/COUNT(B12:D12), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F12">
@@ -1070,45 +1140,49 @@
         <v>0</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J12" s="3">
         <v>0</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q12" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S12" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U12" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W12" s="3">
         <v>7.2541316770242101</v>
       </c>
-      <c r="T12" s="2">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
       <c r="X12" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="E13" s="2" t="str">
-        <f>IF(COUNT(B13:D13) &lt;&gt; 0, SUM(B13:D13)/COUNT(B13:D13), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F13">
@@ -1121,42 +1195,46 @@
         <v>0</v>
       </c>
       <c r="I13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M13" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q13" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="T13" s="5">
-        <v>0</v>
-      </c>
-      <c r="U13" t="s">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U13" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X13" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="s">
         <v>2</v>
       </c>
-      <c r="V13" t="s">
+      <c r="Z13" t="s">
         <v>2</v>
       </c>
-      <c r="W13" t="s">
+      <c r="AA13" t="s">
         <v>2</v>
       </c>
-      <c r="X13" t="s">
+      <c r="AB13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="E14" s="2" t="str">
-        <f>IF(COUNT(B14:D14) &lt;&gt; 0, SUM(B14:D14)/COUNT(B14:D14), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F14">
@@ -1169,42 +1247,46 @@
         <v>1</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M14" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q14" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S14" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U14" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W14" s="3">
         <v>247165752</v>
       </c>
-      <c r="T14" s="2">
-        <v>1</v>
-      </c>
-      <c r="U14">
-        <v>1</v>
-      </c>
-      <c r="V14">
-        <v>1</v>
-      </c>
-      <c r="W14">
-        <v>1</v>
-      </c>
       <c r="X14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="Z14">
+        <v>1</v>
+      </c>
+      <c r="AA14">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="E15" s="2" t="str">
-        <f>IF(COUNT(B15:D15) &lt;&gt; 0, SUM(B15:D15)/COUNT(B15:D15), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F15">
@@ -1217,42 +1299,46 @@
         <v>1</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M15" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q15" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S15" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U15" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W15" s="3">
         <v>8</v>
       </c>
-      <c r="T15" s="2">
-        <v>1</v>
-      </c>
-      <c r="U15">
-        <v>1</v>
-      </c>
-      <c r="V15">
-        <v>1</v>
-      </c>
-      <c r="W15">
-        <v>1</v>
-      </c>
       <c r="X15" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>1</v>
+      </c>
+      <c r="AA15">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="E16" s="2" t="str">
-        <f>IF(COUNT(B16:D16) &lt;&gt; 0, SUM(B16:D16)/COUNT(B16:D16), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F16">
@@ -1265,42 +1351,46 @@
         <v>1</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M16" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q16" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S16" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U16" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W16" s="3">
         <v>10405071392</v>
       </c>
-      <c r="T16" s="2">
-        <v>1</v>
-      </c>
-      <c r="U16">
-        <v>1</v>
-      </c>
-      <c r="V16">
-        <v>1</v>
-      </c>
-      <c r="W16">
-        <v>1</v>
-      </c>
       <c r="X16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y16">
+        <v>1</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="E17" s="2" t="str">
-        <f>IF(COUNT(B17:D17) &lt;&gt; 0, SUM(B17:D17)/COUNT(B17:D17), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F17">
@@ -1313,43 +1403,47 @@
         <v>0</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M17" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q17" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S17" s="3">
-        <v>0</v>
-      </c>
-      <c r="T17" s="2">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U17" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W17" s="3">
+        <v>0</v>
+      </c>
+      <c r="X17" s="2">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="U17">
-        <v>0</v>
-      </c>
-      <c r="V17">
-        <v>0</v>
-      </c>
-      <c r="W17">
-        <v>1</v>
-      </c>
-      <c r="X17" s="2">
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="2">
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="E18" s="2" t="str">
-        <f>IF(COUNT(B18:D18) &lt;&gt; 0, SUM(B18:D18)/COUNT(B18:D18), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F18">
@@ -1362,42 +1456,46 @@
         <v>1</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M18" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q18" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S18" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U18" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W18" s="3">
         <v>5</v>
       </c>
-      <c r="T18" s="2">
-        <v>1</v>
-      </c>
-      <c r="U18">
-        <v>1</v>
-      </c>
-      <c r="V18">
-        <v>1</v>
-      </c>
-      <c r="W18">
-        <v>1</v>
-      </c>
       <c r="X18" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+      <c r="AA18">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="E19" s="2" t="str">
-        <f>IF(COUNT(B19:D19) &lt;&gt; 0, SUM(B19:D19)/COUNT(B19:D19), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F19">
@@ -1410,37 +1508,41 @@
         <v>0</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M19" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q19" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S19" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U19" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W19" s="3">
         <v>1.8409533159662601</v>
       </c>
-      <c r="T19" s="2">
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>0</v>
-      </c>
-      <c r="V19">
-        <v>0</v>
-      </c>
-      <c r="W19">
-        <v>0</v>
-      </c>
       <c r="X19" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1448,46 +1550,59 @@
         <v>1</v>
       </c>
       <c r="E20" s="2">
-        <f>IF(COUNT(B20:D20) &lt;&gt; 0, SUM(B20:D20)/COUNT(B20:D20), "-%")</f>
-        <v>1</v>
-      </c>
-      <c r="I20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-%</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M20" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q20" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S20" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U20" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W20" s="3">
         <v>5</v>
       </c>
-      <c r="T20" s="2">
-        <v>0</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
-      <c r="V20">
-        <v>0</v>
-      </c>
-      <c r="W20">
-        <v>0</v>
-      </c>
       <c r="X20" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="E21" s="2" t="str">
-        <f>IF(COUNT(B21:D21) &lt;&gt; 0, SUM(B21:D21)/COUNT(B21:D21), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F21">
@@ -1496,91 +1611,105 @@
       <c r="G21">
         <v>0</v>
       </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
       <c r="I21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M21" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q21" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S21" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U21" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W21" s="3">
         <v>5</v>
       </c>
-      <c r="T21" s="2">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-      <c r="W21">
-        <v>0</v>
-      </c>
       <c r="X21" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="E22" s="2" t="str">
-        <f>IF(COUNT(B22:D22) &lt;&gt; 0, SUM(B22:D22)/COUNT(B22:D22), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
         <v>1</v>
       </c>
       <c r="H22">
         <v>0.5</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="0"/>
-        <v>0.75</v>
+        <f t="shared" si="1"/>
+        <v>0.83333333333333337</v>
       </c>
       <c r="M22" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q22" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S22" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U22" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W22" s="3">
         <v>65</v>
       </c>
-      <c r="T22" s="2">
-        <v>1</v>
-      </c>
-      <c r="U22">
-        <v>1</v>
-      </c>
-      <c r="V22">
-        <v>1</v>
-      </c>
-      <c r="W22">
-        <v>1</v>
-      </c>
       <c r="X22" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y22">
+        <v>1</v>
+      </c>
+      <c r="Z22">
+        <v>1</v>
+      </c>
+      <c r="AA22">
+        <v>1</v>
+      </c>
+      <c r="AB22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="D23" s="3">
+      <c r="C23" s="3">
         <v>0</v>
       </c>
       <c r="E23" s="2">
-        <f>IF(COUNT(B23:D23) &lt;&gt; 0, SUM(B23:D23)/COUNT(B23:D23), "-%")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F23">
@@ -1593,86 +1722,94 @@
         <v>1</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M23" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q23" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S23" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U23" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W23" s="3">
         <v>5</v>
       </c>
-      <c r="T23" s="2">
+      <c r="X23" s="2">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="U23">
-        <v>1</v>
-      </c>
-      <c r="V23">
-        <v>1</v>
-      </c>
-      <c r="W23">
-        <v>0</v>
-      </c>
-      <c r="X23" s="2">
+      <c r="Y23">
+        <v>1</v>
+      </c>
+      <c r="Z23">
+        <v>1</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="2">
         <v>0.66669999999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="E24" s="2" t="str">
-        <f>IF(COUNT(B24:D24) &lt;&gt; 0, SUM(B24:D24)/COUNT(B24:D24), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="H24">
         <v>1</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M24" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q24" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S24" s="3">
-        <v>0</v>
-      </c>
-      <c r="T24" s="2">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U24" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W24" s="3">
+        <v>0</v>
+      </c>
+      <c r="X24" s="2">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="U24">
-        <v>1</v>
-      </c>
-      <c r="V24">
-        <v>0</v>
-      </c>
-      <c r="W24">
-        <v>0</v>
-      </c>
-      <c r="X24" s="2">
+      <c r="Y24">
+        <v>1</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="2">
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>23</v>
       </c>
       <c r="E25" s="2" t="str">
-        <f>IF(COUNT(B25:D25) &lt;&gt; 0, SUM(B25:D25)/COUNT(B25:D25), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F25">
@@ -1685,88 +1822,99 @@
         <v>0</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="M25" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q25" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S25" s="3" t="s">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U25" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="T25" s="5">
-        <v>0</v>
-      </c>
-      <c r="U25" t="s">
+      <c r="X25" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y25" t="s">
         <v>2</v>
       </c>
-      <c r="V25" t="s">
+      <c r="Z25" t="s">
         <v>2</v>
       </c>
-      <c r="W25" t="s">
+      <c r="AA25" t="s">
         <v>2</v>
       </c>
-      <c r="X25" t="s">
+      <c r="AB25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>24</v>
       </c>
       <c r="E26" s="2" t="str">
-        <f>IF(COUNT(B26:D26) &lt;&gt; 0, SUM(B26:D26)/COUNT(B26:D26), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="M26" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q26" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S26" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U26" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W26" s="3">
         <v>-5</v>
       </c>
-      <c r="T26" s="2">
+      <c r="X26" s="2">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="U26">
-        <v>0</v>
-      </c>
-      <c r="V26">
-        <v>0</v>
-      </c>
-      <c r="W26">
-        <v>1</v>
-      </c>
-      <c r="X26" s="2">
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="2">
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="E27" s="2" t="str">
-        <f>IF(COUNT(B27:D27) &lt;&gt; 0, SUM(B27:D27)/COUNT(B27:D27), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F27">
@@ -1779,42 +1927,46 @@
         <v>0</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="M27" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q27" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S27" s="3">
-        <v>1</v>
-      </c>
-      <c r="T27" s="2">
-        <v>0</v>
-      </c>
-      <c r="U27">
-        <v>0</v>
-      </c>
-      <c r="V27">
-        <v>0</v>
-      </c>
-      <c r="W27" t="s">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U27" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W27" s="3">
+        <v>1</v>
+      </c>
+      <c r="X27" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27" t="s">
         <v>2</v>
       </c>
-      <c r="X27" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="AB27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="E28" s="2" t="str">
-        <f>IF(COUNT(B28:D28) &lt;&gt; 0, SUM(B28:D28)/COUNT(B28:D28), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F28">
@@ -1824,42 +1976,46 @@
         <v>1</v>
       </c>
       <c r="I28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M28" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q28" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S28" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U28" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W28" s="3">
         <v>60</v>
       </c>
-      <c r="T28" s="2">
-        <v>1</v>
-      </c>
-      <c r="U28">
-        <v>1</v>
-      </c>
-      <c r="V28">
-        <v>1</v>
-      </c>
-      <c r="W28">
-        <v>1</v>
-      </c>
       <c r="X28" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y28">
+        <v>1</v>
+      </c>
+      <c r="Z28">
+        <v>1</v>
+      </c>
+      <c r="AA28">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="E29" s="2" t="str">
-        <f>IF(COUNT(B29:D29) &lt;&gt; 0, SUM(B29:D29)/COUNT(B29:D29), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="G29">
@@ -1869,42 +2025,46 @@
         <v>1</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="M29" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q29" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S29" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U29" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W29" s="3">
         <v>5</v>
       </c>
-      <c r="T29" s="2">
-        <v>0</v>
-      </c>
-      <c r="U29">
-        <v>0</v>
-      </c>
-      <c r="V29">
-        <v>0</v>
-      </c>
-      <c r="W29">
-        <v>0</v>
-      </c>
       <c r="X29" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>0</v>
+      </c>
+      <c r="AA29">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="E30" s="2" t="str">
-        <f>IF(COUNT(B30:D30) &lt;&gt; 0, SUM(B30:D30)/COUNT(B30:D30), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F30">
@@ -1917,84 +2077,92 @@
         <v>0</v>
       </c>
       <c r="I30" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M30" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q30" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S30" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U30" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W30" s="3">
         <v>10405071407</v>
       </c>
-      <c r="T30" s="2">
-        <v>1</v>
-      </c>
-      <c r="U30">
-        <v>1</v>
-      </c>
-      <c r="V30">
-        <v>1</v>
-      </c>
-      <c r="W30">
-        <v>1</v>
-      </c>
       <c r="X30" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y30">
+        <v>1</v>
+      </c>
+      <c r="Z30">
+        <v>1</v>
+      </c>
+      <c r="AA30">
+        <v>1</v>
+      </c>
+      <c r="AB30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="E31" s="2" t="str">
-        <f>IF(COUNT(B31:D31) &lt;&gt; 0, SUM(B31:D31)/COUNT(B31:D31), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M31" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q31" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S31" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U31" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W31" s="3">
         <v>5</v>
       </c>
-      <c r="T31" s="2">
-        <v>0</v>
-      </c>
-      <c r="U31">
-        <v>0</v>
-      </c>
-      <c r="V31">
-        <v>0</v>
-      </c>
-      <c r="W31">
-        <v>0</v>
-      </c>
       <c r="X31" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y31">
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <v>0</v>
+      </c>
+      <c r="AA31">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A32" s="6">
         <v>30</v>
       </c>
       <c r="E32" s="2" t="str">
-        <f>IF(COUNT(B32:D32) &lt;&gt; 0, SUM(B32:D32)/COUNT(B32:D32), "-%")</f>
+        <f t="shared" si="0"/>
         <v>-%</v>
       </c>
       <c r="F32">
@@ -2007,80 +2175,95 @@
         <v>0</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M32" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-%</v>
       </c>
       <c r="Q32" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>-%</v>
-      </c>
-      <c r="S32" s="3">
+        <f t="shared" si="3"/>
+        <v>-%</v>
+      </c>
+      <c r="U32" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-%</v>
+      </c>
+      <c r="W32" s="3">
         <v>383.61803398875003</v>
       </c>
-      <c r="T32" s="2">
-        <v>0</v>
-      </c>
-      <c r="U32">
-        <v>0</v>
-      </c>
-      <c r="V32">
-        <v>0</v>
-      </c>
-      <c r="W32">
-        <v>0</v>
-      </c>
       <c r="X32" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="2">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="expression" dxfId="14" priority="10">
-      <formula>E1&lt;$T1</formula>
+    <cfRule type="expression" dxfId="14" priority="13">
+      <formula>E1&lt;$X1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="19">
+    <cfRule type="expression" dxfId="13" priority="22">
       <formula>E1="-%"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="22">
-      <formula>E1&gt;$T1</formula>
+    <cfRule type="expression" dxfId="12" priority="25">
+      <formula>E1&gt;$X1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="expression" dxfId="11" priority="7">
-      <formula>I1&lt;$T1</formula>
+    <cfRule type="expression" dxfId="11" priority="10">
+      <formula>I1&lt;$X1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>I1="-%"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9">
-      <formula>I1&gt;$T1</formula>
+    <cfRule type="expression" dxfId="9" priority="12">
+      <formula>I1&gt;$X1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>M1&lt;$T1</formula>
+    <cfRule type="expression" dxfId="8" priority="7">
+      <formula>M1&lt;$X1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>M1="-%"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>M1&gt;$T1</formula>
+    <cfRule type="expression" dxfId="6" priority="9">
+      <formula>M1&gt;$X1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576">
+    <cfRule type="expression" dxfId="5" priority="4">
+      <formula>Q1&lt;$X1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>Q1="-%"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>Q1&gt;$X1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U1:U1048576">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>Q1&lt;$T1</formula>
+      <formula>U1&lt;$X1</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>Q1="-%"</formula>
+      <formula>U1="-%"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>Q1&gt;$T1</formula>
+      <formula>U1&gt;$X1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>